<commit_message>
Built the tree and trying to call things recursively but it breaks for some reason I figured I would save my work
</commit_message>
<xml_diff>
--- a/DecisionTree/Decision Tree (Loan).xlsx
+++ b/DecisionTree/Decision Tree (Loan).xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adammcpherson/Documents/Machine/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adammcpherson/Documents/Machine/DecisionTree/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{29C0EEAE-1194-E848-BC3A-83E01FF4C351}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{29C0EEAE-1194-E848-BC3A-83E01FF4C351}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="25">
   <si>
     <t>Credit</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>Weigthed Entropy</t>
   </si>
 </sst>
 </file>
@@ -228,7 +231,7 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -247,6 +250,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -567,11 +576,12 @@
   <dimension ref="A1:AA26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="9" max="9" width="18.83203125" customWidth="1"/>
     <col min="10" max="10" width="16.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -630,7 +640,7 @@
         <f>4/12</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="11">
         <f>G2*H2</f>
         <v>0.27042604148637761</v>
       </c>
@@ -664,7 +674,7 @@
         <f t="shared" ref="H3:H4" si="2">4/12</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="11">
         <f t="shared" ref="I3:I4" si="3">G3*H3</f>
         <v>0.33333333333333331</v>
       </c>
@@ -715,7 +725,7 @@
         <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="11">
         <f t="shared" si="3"/>
         <v>0.27042604148637761</v>
       </c>
@@ -741,7 +751,7 @@
       <c r="H5" t="s">
         <v>14</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="11">
         <f>SUM(I2:I4)</f>
         <v>0.87418541630608859</v>
       </c>
@@ -786,8 +796,8 @@
       <c r="H6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>10</v>
+      <c r="I6" s="12" t="s">
+        <v>24</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>15</v>
@@ -853,7 +863,7 @@
         <f>6/12</f>
         <v>0.5</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I7" s="12">
         <f>G7*H7</f>
         <v>0.32501121082417705</v>
       </c>
@@ -918,7 +928,7 @@
         <f>6/12</f>
         <v>0.5</v>
       </c>
-      <c r="I8" s="1">
+      <c r="I8" s="12">
         <f t="shared" ref="I8" si="6">G8*H8</f>
         <v>0.32501121082417705</v>
       </c>
@@ -958,7 +968,7 @@
       <c r="H9" t="s">
         <v>14</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="11">
         <f>SUM(I7:I8)</f>
         <v>0.65002242164835411</v>
       </c>
@@ -1017,7 +1027,7 @@
       <c r="H10" t="s">
         <v>11</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="11" t="s">
         <v>10</v>
       </c>
       <c r="J10" s="2" t="s">
@@ -1075,7 +1085,7 @@
         <f>6/12</f>
         <v>0.5</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="11">
         <f>G11*H11</f>
         <v>0.45914791702724478</v>
       </c>
@@ -1140,7 +1150,7 @@
         <f>6/12</f>
         <v>0.5</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="11">
         <f t="shared" ref="I12" si="13">G12*H12</f>
         <v>0.45914791702724478</v>
       </c>
@@ -1181,7 +1191,7 @@
       <c r="H13" t="s">
         <v>14</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="11">
         <f>SUM(I11:I12)</f>
         <v>0.91829583405448956</v>
       </c>

</xml_diff>

<commit_message>
Fixed the bug of incorrect rows
</commit_message>
<xml_diff>
--- a/DecisionTree/Decision Tree (Loan).xlsx
+++ b/DecisionTree/Decision Tree (Loan).xlsx
@@ -576,7 +576,7 @@
   <dimension ref="A1:AA26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -997,7 +997,7 @@
         <v>1</v>
       </c>
       <c r="Q9" s="1">
-        <f t="shared" si="9"/>
+        <f>M9/SUM($M$7:$M$9)</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="R9" s="1">

</xml_diff>

<commit_message>
Works with Iris dataset
</commit_message>
<xml_diff>
--- a/DecisionTree/Decision Tree (Loan).xlsx
+++ b/DecisionTree/Decision Tree (Loan).xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="27">
   <si>
     <t>Credit</t>
   </si>
@@ -99,6 +99,12 @@
   </si>
   <si>
     <t>Weigthed Entropy</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
@@ -576,7 +582,7 @@
   <dimension ref="A1:AA26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -735,8 +741,8 @@
       <c r="T4" s="3">
         <v>1</v>
       </c>
-      <c r="U4" s="1">
-        <v>0</v>
+      <c r="U4" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="V4" s="1">
         <v>2</v>
@@ -761,8 +767,8 @@
       <c r="T5" s="1">
         <v>0</v>
       </c>
-      <c r="U5" s="3">
-        <v>1</v>
+      <c r="U5" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="V5" s="1">
         <v>2</v>
@@ -956,7 +962,7 @@
         <v>0</v>
       </c>
       <c r="Q8" s="1">
-        <f t="shared" ref="Q8:Q9" si="9">M8/SUM($M$7:$M$9)</f>
+        <f t="shared" ref="Q8" si="9">M8/SUM($M$7:$M$9)</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="R8" s="1">

</xml_diff>